<commit_message>
add some missing part in the file
</commit_message>
<xml_diff>
--- a/src/ontology/immunology/TLR3.xlsx
+++ b/src/ontology/immunology/TLR3.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="26800" yWindow="3680" windowWidth="32420" windowHeight="19060" tabRatio="500"/>
+    <workbookView xWindow="660" yWindow="2000" windowWidth="21600" windowHeight="14400" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="TRIF" sheetId="1" r:id="rId1"/>
@@ -19,90 +19,268 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="105">
+  <si>
+    <t>Interferon regulatory factor-3-mediated activation of the interferon-sensitive response element by Toll-like receptor (TLR) 4 but not TLR3 requires the p65 subunit of NF-kappa.</t>
+  </si>
+  <si>
+    <t>PMID: 14557267</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IRF3pIRF3p translocate to nucleus </t>
+  </si>
+  <si>
+    <t>Virus-Dependent Phosphorylation of the IRF-3 Transcription Factor Regulates Nuclear Translocation, Transactivation Potential, and Proteasome-Mediated Degradation</t>
+  </si>
+  <si>
+    <t>PMID: 9566918</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IRF3p65 translocate to nucleus </t>
+  </si>
+  <si>
+    <t>IRf3pIRF3pISRE</t>
+  </si>
+  <si>
+    <t>2TLR3dsRNATRIF+TRAF3-&gt; 2TLR3dsRNATRIFTRAF3</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>2TLR3dsRNATRIFTRAF3+TBK1-tank-IKKe-&gt;2TLR3dsRNATRIFTRAF3TBK1-tank-IKKe</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>2TLR3dsRNATRIFTRAF3TBK1-tank-IKKe-&gt;2TLR3dsRNATRIFTRAF3+TBK1tank63ubIKKe</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>2TLR3dsRNATRIFTRAF3TBK1-tank-IKKe-&gt;2TLR3dsRNATRIFTRAF3+TBK1tank63ubIKKe</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>IRF7p+IRF7p-&gt;IRF7pIRF7p</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>phom of IR73p</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>phomp locate in cyto</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>IRF3p+IRF3P-&gt; IRF3pIRF3p</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Spreadsheet id</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>About</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Date Created</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Last edited</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Editors</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>handle</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Entities</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Kind</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>class</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>super(s)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>realizes</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>part_of</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>binding domains</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>LRR</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>TIR</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>TRAF</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>protein complex disassembly</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>GO:0043241</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>pcd</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>protein complex assembly</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>process</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>conformational change  of TBK1tankk63ubIKKe</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>GO:0000060</t>
+  </si>
+  <si>
+    <t>protein import into cell nucleus, translocation</t>
+  </si>
+  <si>
+    <t>pint</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>pint located in cyto</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Evidence for</t>
+  </si>
   <si>
     <t>Title</t>
-    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>Evidence Code</t>
-    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>Pubmed id</t>
-    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>URL</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>PMID: 17327220</t>
+  </si>
+  <si>
+    <t>PMID: 12133833</t>
+  </si>
+  <si>
+    <t>Lipopolysaccharide-mediated interferon regulatory factor activation involves TBK1-IKKepsilon-dependent Lys(63)-linked polyubiquitination and phosphorylation of TANK/I-TRAF.</t>
+  </si>
+  <si>
+    <t>PMID: 17823124</t>
+  </si>
+  <si>
+    <t>TBK1tankk63ubIKKe+IRF3-&gt; IRF3p</t>
+  </si>
+  <si>
+    <t>Identification of Ser-386 of interferon regulatory factor 3 as critical target for inducible phosphorylation that determines activation</t>
+  </si>
+  <si>
+    <t>PMID: 14703513</t>
+  </si>
+  <si>
+    <t>IRF3p+IRF3P-&gt; IRF3pIRF3p</t>
+  </si>
+  <si>
+    <t>IRF3p+p65-&gt;IRF3p65</t>
   </si>
   <si>
     <t>processes</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>2TLR3+dsRNA-&gt; 2TLR3dsRNA</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>2TLR3dsRNA+TRIF-&gt;2TLR3dsRNATRIF</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>TLR3</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>2TLR3</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>dsRNA</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t xml:space="preserve">Uses entities from </t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>TLR3-01</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>dsRNA recognition and signaling via TLR3</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>TLR4-01</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>TLR4-03</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>cellular protein complex assembly</t>
   </si>
   <si>
     <t>process</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>GO:0043623</t>
   </si>
   <si>
     <t>Cpca</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>protein complex assembly</t>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>GO:0006461</t>
   </si>
   <si>
     <t>pca</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>trafdbp located in early endosome</t>
@@ -118,203 +296,119 @@
   </si>
   <si>
     <t>phom of IRF3p</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>IRF3p+IRF7p-&gt;IRF3pIRF7p</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>phet of IRF3p and phet of IRF7</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>phetp located in cyto</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>IRF3p+p65-&gt;IRF3p65</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>phet of IRF3p and p65</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t xml:space="preserve">IRF3pIRF3p translocate to nucleus  </t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>nlsb of IRF3pIRF3p</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t xml:space="preserve">IRF3p65 translocate to nuc </t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>nlsb of IRF3pp65</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>IRF7pIRF7p translocate  to nuc</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>nlsb of IRF7pIRF7p</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>IRF3pIRF7p translocate to nuc</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>nlsb of IRF3pIRF7p</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>IRF3pIRF3p+ISREdnas-&gt;IRF3pIRF3pISREdnas</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t xml:space="preserve">ISREb of IRF3pIRF3p  </t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>pDca</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>IRF3pIRF3p</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>tf and RPIITFAEB and ssDb of IRF3pIRF3p</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>TRPIIP</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>2TLR3dsRNATRIFTRAF3+TBK1-tank-IKKe-&gt;2TLR3dsRNATRIFTRAF3TBK1-tank-IKKe</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>2TLR3dsRNATRIFTRAF3TBK1-tank-IKKe-&gt;2TLR3dsRNATRIFTRAF3+TBK1tank63ubIKKe</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>2TLR3dsRNATRIF+TRAF3-&gt; 2TLR3dsRNATRIFTRAF3</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>sf of TBK1tankk63ubIKKe</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>pcd loated in cyto</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>TBK1tankk63ubIKKe+IRF3-&gt; IRF3p</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>KD of TBK and IKKe part of TBK1tankk63ubIKKe and KB of IRF-3</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>pop located in cyto</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>TBK1tankk63ubIKKe+IRF7-&gt; IRF7p</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>KD of TBK and IKKe part of TBK1tankk63ubIKKe and KB of IRF-7</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>IRF7p+IRF7p-&gt;IRF7pIRF7p</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>phom of IR73p</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>phomp locate in cyto</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>IRF3p+IRF3P-&gt; IRF3pIRF3p</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Spreadsheet id</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>About</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Date Created</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Last edited</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Editors</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>handle</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Entities</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Kind</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>class</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>super(s)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>realizes</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>part_of</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>binding domains</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>complexes without process forming them</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>has_part</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Evidence for</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -327,8 +421,13 @@
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
+      <sz val="10"/>
+      <name val="Verdana"/>
+    </font>
+    <font>
+      <b/>
       <sz val="10"/>
       <name val="Verdana"/>
     </font>
@@ -420,15 +519,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -451,6 +550,15 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -782,10 +890,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <dimension ref="A1:G69"/>
+  <dimension ref="A1:G40"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -800,29 +908,29 @@
   <sheetData>
     <row r="1" spans="1:7" s="9" customFormat="1">
       <c r="A1" s="1" t="s">
-        <v>60</v>
+        <v>15</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>61</v>
+        <v>16</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>62</v>
+        <v>17</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>63</v>
+        <v>18</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>64</v>
+        <v>19</v>
       </c>
       <c r="F1" s="4"/>
       <c r="G1" s="4"/>
     </row>
     <row r="2" spans="1:7" ht="39">
       <c r="A2" s="5" t="s">
-        <v>11</v>
+        <v>62</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>12</v>
+        <v>63</v>
       </c>
       <c r="C2" s="7">
         <v>38707</v>
@@ -836,13 +944,13 @@
     </row>
     <row r="3" spans="1:7" ht="26">
       <c r="A3" s="4" t="s">
-        <v>10</v>
+        <v>61</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>13</v>
+        <v>64</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>14</v>
+        <v>65</v>
       </c>
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
@@ -850,25 +958,25 @@
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="1" t="s">
-        <v>65</v>
+        <v>20</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>66</v>
+        <v>21</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>67</v>
+        <v>22</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>68</v>
+        <v>23</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>69</v>
+        <v>24</v>
       </c>
       <c r="F4" s="6"/>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="4" t="s">
-        <v>7</v>
+        <v>58</v>
       </c>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
@@ -878,7 +986,7 @@
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="4" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
@@ -888,7 +996,7 @@
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="4" t="s">
-        <v>9</v>
+        <v>60</v>
       </c>
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
@@ -898,135 +1006,157 @@
     </row>
     <row r="8" spans="1:7" ht="26">
       <c r="A8" s="4" t="s">
-        <v>18</v>
+        <v>69</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>15</v>
+        <v>66</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>16</v>
+        <v>67</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>17</v>
+        <v>68</v>
       </c>
       <c r="E8" s="4"/>
       <c r="F8" s="6"/>
     </row>
     <row r="9" spans="1:7" ht="26">
       <c r="A9" s="4" t="s">
-        <v>21</v>
+        <v>71</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>19</v>
+        <v>34</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>16</v>
+        <v>67</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>20</v>
+        <v>70</v>
       </c>
       <c r="E9" s="4"/>
       <c r="F9" s="6"/>
     </row>
     <row r="10" spans="1:7" ht="26">
-      <c r="A10" s="4"/>
-      <c r="B10" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>68</v>
-      </c>
+      <c r="A10" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E10" s="4"/>
       <c r="F10" s="6"/>
-      <c r="G10" s="1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7">
-      <c r="A11" s="4"/>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
+    </row>
+    <row r="11" spans="1:7" ht="39">
+      <c r="A11" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>37</v>
+      </c>
       <c r="E11" s="4"/>
       <c r="F11" s="6"/>
     </row>
     <row r="12" spans="1:7" ht="26">
       <c r="A12" s="4"/>
-      <c r="B12" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
+      <c r="B12" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>23</v>
+      </c>
       <c r="F12" s="6"/>
+      <c r="G12" s="1" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="13" spans="1:7" ht="26">
       <c r="A13" s="4"/>
       <c r="B13" s="4" t="s">
-        <v>6</v>
+        <v>56</v>
       </c>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
       <c r="F13" s="6"/>
-    </row>
-    <row r="14" spans="1:7" ht="52">
+      <c r="G13" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="26">
       <c r="A14" s="4"/>
       <c r="B14" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>22</v>
-      </c>
+        <v>57</v>
+      </c>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
       <c r="E14" s="4"/>
-      <c r="F14" s="10"/>
-    </row>
-    <row r="15" spans="1:7" ht="78">
+      <c r="F14" s="6"/>
+      <c r="G14" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="52">
       <c r="A15" s="4"/>
       <c r="B15" s="4" t="s">
-        <v>46</v>
+        <v>98</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>25</v>
+        <v>74</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>23</v>
+        <v>72</v>
       </c>
       <c r="E15" s="4"/>
-      <c r="F15" s="6"/>
-    </row>
-    <row r="16" spans="1:7" ht="65">
+      <c r="F15" s="10"/>
+      <c r="G15" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="78">
       <c r="A16" s="4"/>
       <c r="B16" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="C16" s="11" t="s">
-        <v>49</v>
+        <v>96</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>75</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>50</v>
+        <v>73</v>
       </c>
       <c r="E16" s="4"/>
       <c r="F16" s="6"/>
+      <c r="G16" s="4" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="17" spans="1:6" ht="65">
       <c r="A17" s="4"/>
       <c r="B17" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>52</v>
+        <v>97</v>
+      </c>
+      <c r="C17" s="11" t="s">
+        <v>36</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>53</v>
+        <v>99</v>
       </c>
       <c r="E17" s="4"/>
       <c r="F17" s="6"/>
@@ -1034,27 +1164,27 @@
     <row r="18" spans="1:6" ht="65">
       <c r="A18" s="4"/>
       <c r="B18" s="4" t="s">
-        <v>54</v>
+        <v>100</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>55</v>
+        <v>101</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>53</v>
+        <v>102</v>
       </c>
       <c r="E18" s="4"/>
       <c r="F18" s="6"/>
     </row>
-    <row r="19" spans="1:6" ht="26">
+    <row r="19" spans="1:6" ht="65">
       <c r="A19" s="4"/>
       <c r="B19" s="4" t="s">
-        <v>56</v>
+        <v>103</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>57</v>
+        <v>104</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>58</v>
+        <v>102</v>
       </c>
       <c r="E19" s="4"/>
       <c r="F19" s="6"/>
@@ -1062,13 +1192,13 @@
     <row r="20" spans="1:6" ht="26">
       <c r="A20" s="4"/>
       <c r="B20" s="4" t="s">
-        <v>59</v>
+        <v>11</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>58</v>
+        <v>13</v>
       </c>
       <c r="E20" s="4"/>
       <c r="F20" s="6"/>
@@ -1076,13 +1206,13 @@
     <row r="21" spans="1:6" ht="26">
       <c r="A21" s="4"/>
       <c r="B21" s="4" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>28</v>
+        <v>76</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>29</v>
+        <v>13</v>
       </c>
       <c r="E21" s="4"/>
       <c r="F21" s="6"/>
@@ -1090,75 +1220,83 @@
     <row r="22" spans="1:6" ht="26">
       <c r="A22" s="4"/>
       <c r="B22" s="4" t="s">
-        <v>30</v>
+        <v>77</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>31</v>
+        <v>78</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>29</v>
+        <v>79</v>
       </c>
       <c r="E22" s="4"/>
       <c r="F22" s="6"/>
     </row>
-    <row r="23" spans="1:6" ht="39">
+    <row r="23" spans="1:6" ht="26">
       <c r="A23" s="4"/>
       <c r="B23" s="4" t="s">
-        <v>32</v>
+        <v>80</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D23" s="4"/>
+        <v>81</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>79</v>
+      </c>
       <c r="E23" s="4"/>
       <c r="F23" s="6"/>
     </row>
-    <row r="24" spans="1:6" ht="26">
+    <row r="24" spans="1:6" ht="39">
       <c r="A24" s="4"/>
       <c r="B24" s="4" t="s">
-        <v>34</v>
+        <v>82</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="D24" s="4"/>
+        <v>83</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>40</v>
+      </c>
       <c r="E24" s="4"/>
       <c r="F24" s="6"/>
     </row>
     <row r="25" spans="1:6" ht="26">
       <c r="A25" s="4"/>
       <c r="B25" s="4" t="s">
-        <v>36</v>
+        <v>84</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="D25" s="4"/>
+        <v>85</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>40</v>
+      </c>
       <c r="E25" s="4"/>
       <c r="F25" s="6"/>
     </row>
     <row r="26" spans="1:6" ht="26">
       <c r="A26" s="4"/>
       <c r="B26" s="4" t="s">
-        <v>38</v>
+        <v>86</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="D26" s="4"/>
+        <v>87</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>40</v>
+      </c>
       <c r="E26" s="4"/>
       <c r="F26" s="6"/>
     </row>
-    <row r="27" spans="1:6" ht="52">
+    <row r="27" spans="1:6" ht="26">
       <c r="A27" s="4"/>
       <c r="B27" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="D27" s="4" t="s">
         <v>40</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="D27" s="4" t="s">
-        <v>42</v>
       </c>
       <c r="E27" s="4"/>
       <c r="F27" s="6"/>
@@ -1166,232 +1304,152 @@
     <row r="28" spans="1:6" ht="52">
       <c r="A28" s="4"/>
       <c r="B28" s="4" t="s">
-        <v>43</v>
+        <v>90</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>44</v>
+        <v>91</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>45</v>
+        <v>92</v>
       </c>
       <c r="E28" s="4"/>
       <c r="F28" s="6"/>
     </row>
-    <row r="29" spans="1:6">
+    <row r="29" spans="1:6" ht="52">
       <c r="A29" s="4"/>
-      <c r="B29" s="4"/>
-      <c r="C29" s="4"/>
-      <c r="D29" s="4"/>
+      <c r="B29" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>95</v>
+      </c>
       <c r="E29" s="4"/>
       <c r="F29" s="6"/>
     </row>
     <row r="30" spans="1:6">
-      <c r="A30" s="4"/>
-      <c r="B30" s="4"/>
-      <c r="C30" s="4"/>
-      <c r="D30" s="4"/>
-      <c r="E30" s="4"/>
+      <c r="A30" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="B30" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="C30" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="D30" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>45</v>
+      </c>
       <c r="F30" s="6"/>
     </row>
-    <row r="31" spans="1:6">
-      <c r="A31" s="4"/>
-      <c r="B31" s="4"/>
-      <c r="C31" s="4"/>
-      <c r="D31" s="4"/>
-      <c r="E31" s="4"/>
+    <row r="31" spans="1:6" ht="52">
+      <c r="A31" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B31" s="13"/>
+      <c r="C31" s="13"/>
+      <c r="D31" s="13"/>
+      <c r="E31" s="14"/>
       <c r="F31" s="6"/>
     </row>
-    <row r="32" spans="1:6">
-      <c r="A32" s="4"/>
-      <c r="B32" s="4"/>
-      <c r="C32" s="4"/>
-      <c r="D32" s="4"/>
-      <c r="E32" s="4"/>
-      <c r="F32" s="6"/>
-    </row>
-    <row r="33" spans="1:6">
-      <c r="A33" s="4"/>
-      <c r="B33" s="4"/>
-      <c r="C33" s="4"/>
-      <c r="D33" s="4"/>
-      <c r="E33" s="4"/>
-      <c r="F33" s="6"/>
-    </row>
-    <row r="34" spans="1:6">
-      <c r="A34" s="4"/>
-      <c r="B34" s="4"/>
+    <row r="32" spans="1:6" ht="78">
+      <c r="A32" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B32" s="13"/>
+      <c r="C32" s="13"/>
+      <c r="D32" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="E32" s="14" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="78">
+      <c r="A33" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B33" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="C33" s="13"/>
+      <c r="D33" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="E33" s="14"/>
+    </row>
+    <row r="34" spans="1:5" ht="78">
+      <c r="A34" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B34" s="13"/>
       <c r="C34" s="4"/>
-      <c r="D34" s="4"/>
-      <c r="E34" s="4"/>
-      <c r="F34" s="6"/>
-    </row>
-    <row r="35" spans="1:6">
-      <c r="A35" s="4"/>
-      <c r="B35" s="4"/>
-      <c r="C35" s="4"/>
-      <c r="D35" s="4"/>
-      <c r="E35" s="4"/>
-      <c r="F35" s="6"/>
-    </row>
-    <row r="36" spans="1:6">
-      <c r="A36" s="4"/>
-      <c r="B36" s="4"/>
-      <c r="C36" s="4"/>
-      <c r="D36" s="4"/>
-      <c r="E36" s="4"/>
-      <c r="F36" s="6"/>
-    </row>
-    <row r="37" spans="1:6">
-      <c r="A37" s="4"/>
-      <c r="B37" s="4"/>
-      <c r="C37" s="4"/>
-      <c r="D37" s="4"/>
-      <c r="E37" s="4"/>
-      <c r="F37" s="6"/>
-    </row>
-    <row r="38" spans="1:6">
-      <c r="A38" s="4"/>
-      <c r="B38" s="4"/>
-      <c r="C38" s="4"/>
-      <c r="D38" s="4"/>
-      <c r="E38" s="4"/>
-      <c r="F38" s="6"/>
-    </row>
-    <row r="39" spans="1:6">
-      <c r="A39" s="4"/>
-      <c r="B39" s="4"/>
+      <c r="D34" s="13"/>
+      <c r="E34" s="14"/>
+    </row>
+    <row r="35" spans="1:5" ht="39">
+      <c r="A35" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="26">
+      <c r="A36" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="26">
+      <c r="A37" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="39">
+      <c r="A38" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="39">
+      <c r="A39" s="5" t="s">
+        <v>5</v>
+      </c>
       <c r="C39" s="4"/>
-      <c r="D39" s="4"/>
-      <c r="E39" s="4"/>
-      <c r="F39" s="6"/>
-    </row>
-    <row r="40" spans="1:6" ht="39">
-      <c r="A40" s="4"/>
-      <c r="B40" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="D40" s="4"/>
-      <c r="E40" s="4"/>
-      <c r="F40" s="6"/>
-    </row>
-    <row r="41" spans="1:6">
-      <c r="A41" s="4"/>
-      <c r="B41" s="4"/>
-      <c r="C41" s="4"/>
-      <c r="D41" s="4"/>
-      <c r="E41" s="4"/>
-      <c r="F41" s="6"/>
-    </row>
-    <row r="42" spans="1:6">
-      <c r="A42" s="4"/>
-      <c r="B42" s="4"/>
-      <c r="C42" s="4"/>
-      <c r="D42" s="4"/>
-      <c r="E42" s="4"/>
-      <c r="F42" s="6"/>
-    </row>
-    <row r="43" spans="1:6">
-      <c r="A43" s="4"/>
-      <c r="B43" s="4"/>
-      <c r="C43" s="4"/>
-      <c r="D43" s="4"/>
-      <c r="E43" s="4"/>
-      <c r="F43" s="6"/>
-    </row>
-    <row r="44" spans="1:6">
-      <c r="A44" s="4"/>
-      <c r="B44" s="4"/>
-      <c r="C44" s="4"/>
-      <c r="D44" s="4"/>
-      <c r="E44" s="4"/>
-      <c r="F44" s="6"/>
-    </row>
-    <row r="45" spans="1:6">
-      <c r="A45" s="4"/>
-      <c r="B45" s="4"/>
-      <c r="C45" s="4"/>
-      <c r="D45" s="4"/>
-      <c r="E45" s="4"/>
-      <c r="F45" s="6"/>
-    </row>
-    <row r="46" spans="1:6">
-      <c r="A46" s="4"/>
-      <c r="B46" s="4"/>
-      <c r="C46" s="4"/>
-      <c r="D46" s="4"/>
-      <c r="E46" s="4"/>
-      <c r="F46" s="6"/>
-    </row>
-    <row r="47" spans="1:6">
-      <c r="A47" s="4"/>
-      <c r="B47" s="4"/>
-      <c r="C47" s="4"/>
-      <c r="D47" s="4"/>
-      <c r="E47" s="4"/>
-      <c r="F47" s="6"/>
-    </row>
-    <row r="48" spans="1:6">
-      <c r="A48" s="4"/>
-      <c r="B48" s="4"/>
-      <c r="C48" s="4"/>
-      <c r="D48" s="4"/>
-      <c r="E48" s="4"/>
-      <c r="F48" s="6"/>
-    </row>
-    <row r="49" spans="1:6">
-      <c r="A49" s="4"/>
-      <c r="B49" s="4"/>
-      <c r="C49" s="4"/>
-      <c r="D49" s="4"/>
-      <c r="E49" s="4"/>
-      <c r="F49" s="6"/>
-    </row>
-    <row r="50" spans="1:6">
-      <c r="A50" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="B50" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C50" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D50" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E50" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="F50" s="6"/>
-    </row>
-    <row r="51" spans="1:6" ht="26">
-      <c r="A51" s="4"/>
-      <c r="B51" s="4"/>
-      <c r="C51" s="4"/>
-      <c r="D51" s="4"/>
-      <c r="E51" s="4"/>
-      <c r="F51" s="6"/>
-    </row>
-    <row r="52" spans="1:6" ht="39">
-      <c r="A52" s="4"/>
-      <c r="B52" s="4"/>
-      <c r="C52" s="4"/>
-      <c r="D52" s="4"/>
-      <c r="E52" s="4"/>
-      <c r="F52" s="6"/>
-    </row>
-    <row r="53" spans="1:6" ht="26"/>
-    <row r="54" spans="1:6" ht="26"/>
-    <row r="55" spans="1:6" ht="26"/>
-    <row r="56" spans="1:6" ht="52"/>
-    <row r="57" spans="1:6" ht="52"/>
-    <row r="69" ht="39"/>
+    </row>
+    <row r="40" spans="1:5">
+      <c r="A40" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <sheetCalcPr fullCalcOnLoad="1"/>
-  <phoneticPr fontId="2" type="noConversion"/>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>

</xml_diff>

<commit_message>
fix some complex handles
</commit_message>
<xml_diff>
--- a/src/ontology/immunology/TLR3.xlsx
+++ b/src/ontology/immunology/TLR3.xlsx
@@ -19,7 +19,876 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="288">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="292">
+  <si>
+    <t>2TLR3dsRNATRIFTRF3TBK1tankIKKe+ub-&gt; 2TLR3dsRNATRIFTRF3TBK1tankk63ubIKKe</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>TBK1tankk63ubIKKeIRF3</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>TBK1tankk63ubIKKe+IRF3-&gt;TBK1tankk63ubIKKeIRF3</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>TBK1tankk63ubIKKe+IRF7-&gt;TBK1tankk63ubIKKeIRF7</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>TBK1tankk63ubIKKe+IRF3</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>TBK1tankk63ubIKKeIRF3p</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>TBK1tankk63ubIKKeIRF7</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>TBK1tankk63ubIKKeIRF7p</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>TBK1tankk63ubIKKe+IRF7</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>TBK1tankk63ubIKKeIRF7 where IRF7 is phosphorylated</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>TBK1tankk63ubIKKeIRF3 where IRF3 is phosphorylated</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>TBK1tankk63ubIKKeIRF3-&gt; TBK1tankk63ubIKKeIRF3p</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>pb</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">protein binding </t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>GO:0005515</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>pb of IRF3 and pb of TBK1 in TBK1tankk63ubIKKe</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>pca located in cyto</t>
+  </si>
+  <si>
+    <t>pca located in cyto</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>pb of IRF7 and pb of TBK1 in TBK1tankk63ubIKKe</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> Ka of IKKe in TBK1tankk63ubIKKeIRF7 and Kb of IRF7 in TBK1tankk63ubIKKeIRF7</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>TBK1tankk63ubIKKeIRF7-&gt; TBK1tankk63ubIKKeIRF7p</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>phom of IRF7p</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>pca located in cyto</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>pca located in cyto</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>trafdp located in eendo</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>nlsb</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>nuclear localization sequence binding</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>GO:0008139</t>
+  </si>
+  <si>
+    <t>IRF3pIRF3p+IMPalpha4</t>
+  </si>
+  <si>
+    <t>IRF7pIRF7p+IMPalpha4</t>
+  </si>
+  <si>
+    <t>IRF3pIRF7p+IMPalpha4-&gt;IRF3pIRF7pIMPalpha4</t>
+  </si>
+  <si>
+    <t>IRF3pIRF3pIMPalpha4+ISREdnas-&gt;IRF3pIRF3pISREdnas+IMPalpha4</t>
+  </si>
+  <si>
+    <t>IRF7pIRF7pIMPalpha4+ISREdnas-&gt;IRF7pIRF7pISREdnas+IMPalpha4</t>
+  </si>
+  <si>
+    <t>IRF3pIRF7pIMPalpha4+ISREdnas-&gt;IRF3pIRF7pISREdnas+IMPalpha4</t>
+  </si>
+  <si>
+    <t>IRF3pIRF7p+IMPalpha4</t>
+  </si>
+  <si>
+    <t>TBK1TankIKKe</t>
+  </si>
+  <si>
+    <t>TBK1TankIKKe</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>ANNAFIXME</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>complex</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>PRO:tosubmit</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>double-stranded RNA binding</t>
+  </si>
+  <si>
+    <t>molecular function</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>dsRNAb</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>dsRNAb of TLR3 in 2TLR3</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>GO:0022618</t>
+  </si>
+  <si>
+    <t>RNA-protein complex assembly</t>
+  </si>
+  <si>
+    <t>process</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>2TLR3+dsRNA-&gt; 2TLR3dsRNA</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>2TLR3dsRNA+TRIF-&gt; 2TLR3dsRNATRIF</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>RNApca</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">2TLR3dsRNA </t>
+  </si>
+  <si>
+    <t>2TLR3+dsRNA</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>2TLR3dsRNATRIF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2TLR3dsRNA+trif </t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>2TLR3dsRNATRIF+TRF3-&gt; 2TLR3dsRNATRIFTRF3</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>phet of IRF3p and phet of IRF7P</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>NLSsni</t>
+  </si>
+  <si>
+    <t>IRF7pIRF7p+IMPalpha4-&gt; IRF7pIRF7pIMPalpha4</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>nlsb of IMPalpha4</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>NLS-bearing substrate import into nucleus</t>
+  </si>
+  <si>
+    <t>GO:0006607</t>
+  </si>
+  <si>
+    <t>nlsb of IMPalpha4</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>NLSsni</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>double strand dna sequence         transcript_bound_by_protein</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>double strand dna sequence   bound by protein</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>SO:0000279</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>pDca</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>protein-DNA complex assembly</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>GO:0065004</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>super(s)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>tirdbp that has location endves</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>tirdb of trif and tirdb of TLR3 in 2TLR3dsRNA</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">ISREb of IRF3pIRF7p  </t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>tirdb</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">tir domain binding </t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>function</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>GO:0070976</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>tirdbp</t>
+  </si>
+  <si>
+    <t>tir domain complex assembly</t>
+  </si>
+  <si>
+    <t>GO:0071523</t>
+  </si>
+  <si>
+    <t>ubb</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>ubiquitin binding</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>GO:0043130</t>
+  </si>
+  <si>
+    <t>Kb</t>
+  </si>
+  <si>
+    <t>kinase binding</t>
+  </si>
+  <si>
+    <t>GO:0019900</t>
+  </si>
+  <si>
+    <t>Ka</t>
+  </si>
+  <si>
+    <t>kinase activity</t>
+  </si>
+  <si>
+    <t>GO:0016301</t>
+  </si>
+  <si>
+    <t>sf</t>
+  </si>
+  <si>
+    <t>separeted from</t>
+  </si>
+  <si>
+    <t>quality</t>
+  </si>
+  <si>
+    <t>PATO:0001505</t>
+  </si>
+  <si>
+    <t>KD</t>
+  </si>
+  <si>
+    <t>kinase domain</t>
+  </si>
+  <si>
+    <t>Ka of IKKe in TBK1tankk63ubIKKeIRF3 and Kb of IRF3 in TBK1tankk63ubIKKeIRF3</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>TBK1tankk63ubIKKeIRF3p-&gt; TBK1tankk63ubIKKe+IRF3p</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">2TLR3dsRNATRIFTRF3TBK1tankIKKe </t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>TBK1tankk63ubIKKeIRF7p-&gt; TBK1tankk63ubIKKe+IRF7p</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>PMID: 17327220   12133833</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>2TLR3dsRNATRIFTRF3TBK1tankk63ubIKKe</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>2TLR3dsRNATRIFTRF3+TBK1tankIKKe-&gt;2TLR3dsRNATRIFTRF3TBK1tankIKKe</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>rlps2-tt-trf3+TANKK63ub</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>TBK1tankk63ubIKKe</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>TBK1-Tank-IKKe, tank in the complex is  ubiquitinated</t>
+  </si>
+  <si>
+    <t>trafdb</t>
+  </si>
+  <si>
+    <t>traf domain binding</t>
+  </si>
+  <si>
+    <t>molecular function</t>
+  </si>
+  <si>
+    <t>GO:2880558</t>
+  </si>
+  <si>
+    <t>phom</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>protein homodimerization activity</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>molecular function</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>GO:0042803</t>
+  </si>
+  <si>
+    <t>GO:0046982</t>
+  </si>
+  <si>
+    <t>TBK1tankk63ubIKKe+IRF3-&gt; IRF3p</t>
+  </si>
+  <si>
+    <t>Anna Maria</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>PRO:000001154</t>
+  </si>
+  <si>
+    <t>toll-like receptor 3</t>
+  </si>
+  <si>
+    <t>TLR3+TLR3</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>protein complex</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>SO:0001169</t>
+  </si>
+  <si>
+    <t>ds_RNA_viral_sequence</t>
+  </si>
+  <si>
+    <t>nucleic acid</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>trif</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>TRIF</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Gene Product</t>
+  </si>
+  <si>
+    <t>PRO:000001749</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Trf3</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>TRAF 3</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>PRO:000002289</t>
+  </si>
+  <si>
+    <t>TANK</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>PRO:submitted</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>TBK1</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>PRO:000001779</t>
+  </si>
+  <si>
+    <t>IKKe</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>IKK-E</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>PRO:000001778</t>
+  </si>
+  <si>
+    <t>IRF3</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>IRF-3</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>PRO:000002045</t>
+  </si>
+  <si>
+    <t>2TLR3dsRNATRIFTRF3TBK1-tank-IKKe where tank is k63 ubiquitinated</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>post transcriptional modification</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">ub </t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>ubiquitin</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>gene product</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>PRO:000016963</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ISREb of IRF7pIRF7p  </t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>2TLR3dsRNATRIFTRF3</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>2TLR3dsRNATRIF+TRF3</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">2TLR3dsRNATRIFTRF3+TBK1-tank-IKKe </t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Interferon regulatory factor-3-mediated activation of the interferon-sensitive response element by Toll-like receptor (TLR) 4 but not TLR3 requires the p65 subunit of NF-kappa.</t>
+  </si>
+  <si>
+    <t>PMID: 14557267</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IRF3pIRF3p translocate to nucleus </t>
+  </si>
+  <si>
+    <t>IRF3pIRF3p+IMPalpha4-&gt; IRF3pIRF3pIMPalpha4</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>complexes without process forming them</t>
+  </si>
+  <si>
+    <t>has_part</t>
+  </si>
+  <si>
+    <t>TBK1+tank+IKKe</t>
+  </si>
+  <si>
+    <t>pdsb</t>
+  </si>
+  <si>
+    <t>IRF3pIRF7pISREdnas</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>IRF7pIRF7p+ISREdnas</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>IRF7pIRF7pISREdnas</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>2TLR3dsRNATRIFTRF3TBK1tankk63ubIKKe-&gt;2TLR3dsRNATRIFTRF3+TBK1tankk63ubIKKe</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>IMPalpha4</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Importina alpha 4</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>PRO:000009435</t>
+  </si>
+  <si>
+    <t>IRF3pIRF7pIMPalpha4</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>GO:0003725</t>
+  </si>
+  <si>
+    <t>2TLR3dsRNATRIFTRAF3+TBK1-tank-IKKe-&gt;2TLR3dsRNATRIFTRAF3TBK1-tank-IKKe</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>2TLR3dsRNATRIFTRAF3TBK1-tank-IKKe-&gt;2TLR3dsRNATRIFTRAF3+TBK1tank63ubIKKe</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>2TLR3dsRNATRIFTRAF3TBK1-tank-IKKe-&gt;2TLR3dsRNATRIFTRAF3+TBK1tank63ubIKKe</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>IRF7p+IRF7p-&gt;IRF7pIRF7p</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>phomp locate in cyto</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>IRF3p+IRF3P-&gt; IRF3pIRF3p</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Spreadsheet id</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>About</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Date Created</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Last edited</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Editors</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>handle</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Entities</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Kind</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>class</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>super(s)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>realizes</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>part_of</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>binding domains</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>LRR</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>TIR</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>TRAF</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>protein complex disassembly</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>GO:0043241</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>pcd</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>protein complex assembly</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>trafdb of trif in 2TLR3dsRNATRIF</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>pcd loated in cyto</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>TBK1/IKKi-binding domain</t>
+  </si>
+  <si>
+    <t>process</t>
+  </si>
+  <si>
+    <t>phet</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>protein heterodimerization activity</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>molecular function</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>ISREb</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>ISRE binding activity</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>GO:submitted</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>zf TFD</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>traf domain</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>domain</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>PF:02176</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>TBD</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>PF:12845</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>phomp</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>regulation of protein homodimerization activity</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>process</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>process</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>GO:0000060</t>
+  </si>
+  <si>
+    <t>protein import into cell nucleus, translocation</t>
+  </si>
+  <si>
+    <t>pint</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Evidence for</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>Evidence Code</t>
+  </si>
+  <si>
+    <t>Pubmed id</t>
+  </si>
+  <si>
+    <t>URL</t>
+  </si>
+  <si>
+    <t>domain</t>
+  </si>
+  <si>
+    <t>PF00069</t>
+  </si>
+  <si>
+    <t>GO:0043496</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>phetp</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>regulation of protein heterodimerization activity</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>GO:0043497</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>ISREdnas</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>IRF7pIRF7pIMPalpha4</t>
+  </si>
+  <si>
+    <t>IRF3pIRF7p+ISREdnas</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>IRF3pIRF3pISREdnas</t>
+  </si>
+  <si>
+    <t>IRF3pIRF3p+ISREdnas</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>rlps2-tt-trf3</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>rlps2-tt+traf3</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>post transcriptional modification</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>rlps2-tt-trf3-tank63ub</t>
+  </si>
   <si>
     <t>Lipopolysaccharide-mediated interferon regulatory factor activation involves TBK1-IKKepsilon-dependent Lys(63)-linked polyubiquitination and phosphorylation of TANK/I-TRAF.</t>
   </si>
@@ -224,860 +1093,6 @@
   <si>
     <t>2TLR3dsRNATRIF+TRAF3-&gt; 2TLR3dsRNATRIFTRAF3</t>
     <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>2TLR3dsRNATRIFTRAF3+TBK1-tank-IKKe-&gt;2TLR3dsRNATRIFTRAF3TBK1-tank-IKKe</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>2TLR3dsRNATRIFTRAF3TBK1-tank-IKKe-&gt;2TLR3dsRNATRIFTRAF3+TBK1tank63ubIKKe</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>2TLR3dsRNATRIFTRAF3TBK1-tank-IKKe-&gt;2TLR3dsRNATRIFTRAF3+TBK1tank63ubIKKe</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>IRF7p+IRF7p-&gt;IRF7pIRF7p</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>phomp locate in cyto</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>IRF3p+IRF3P-&gt; IRF3pIRF3p</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>Spreadsheet id</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>About</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>Date Created</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>Last edited</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>Editors</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>handle</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>Entities</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>Kind</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>class</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>super(s)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>realizes</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>part_of</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>binding domains</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>LRR</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>TIR</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>TRAF</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>protein complex disassembly</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>GO:0043241</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>pcd</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>protein complex assembly</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>trafdb of trif in 2TLR3dsRNATRIF</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>pcd loated in cyto</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>TBK1/IKKi-binding domain</t>
-  </si>
-  <si>
-    <t>process</t>
-  </si>
-  <si>
-    <t>phet</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>protein heterodimerization activity</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>molecular function</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>ISREb</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>ISRE binding activity</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>GO:submitted</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>zf TFD</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>traf domain</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>domain</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>PF:02176</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>TBD</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>PF:12845</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>phomp</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>regulation of protein homodimerization activity</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>process</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>process</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>GO:0000060</t>
-  </si>
-  <si>
-    <t>protein import into cell nucleus, translocation</t>
-  </si>
-  <si>
-    <t>pint</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>Evidence for</t>
-  </si>
-  <si>
-    <t>Title</t>
-  </si>
-  <si>
-    <t>Evidence Code</t>
-  </si>
-  <si>
-    <t>Pubmed id</t>
-  </si>
-  <si>
-    <t>URL</t>
-  </si>
-  <si>
-    <t>domain</t>
-  </si>
-  <si>
-    <t>PF00069</t>
-  </si>
-  <si>
-    <t>GO:0043496</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>phetp</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>regulation of protein heterodimerization activity</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>GO:0043497</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>ISREdnas</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>IRF7pIRF7pIMPalpha4</t>
-  </si>
-  <si>
-    <t>IRF3pIRF7p+ISREdnas</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>IRF3pIRF3pISREdnas</t>
-  </si>
-  <si>
-    <t>IRF3pIRF3p+ISREdnas</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>rlps2-tt-trf3</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>rlps2-tt+traf3</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>post transcriptional modification</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>rlps2-tt-trf3-tank63ub</t>
-  </si>
-  <si>
-    <t>rlps2-tt-trf3+TANKK63ub</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>TBK1tankk63ubIKKe</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>TBK1-Tank-IKKe, tank in the complex is  ubiquitinated</t>
-  </si>
-  <si>
-    <t>trafdb</t>
-  </si>
-  <si>
-    <t>traf domain binding</t>
-  </si>
-  <si>
-    <t>molecular function</t>
-  </si>
-  <si>
-    <t>GO:2880558</t>
-  </si>
-  <si>
-    <t>phom</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>protein homodimerization activity</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>molecular function</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>GO:0042803</t>
-  </si>
-  <si>
-    <t>GO:0046982</t>
-  </si>
-  <si>
-    <t>TBK1tankk63ubIKKe+IRF3-&gt; IRF3p</t>
-  </si>
-  <si>
-    <t>Anna Maria</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>PRO:000001154</t>
-  </si>
-  <si>
-    <t>toll-like receptor 3</t>
-  </si>
-  <si>
-    <t>TLR3+TLR3</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>protein complex</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>SO:0001169</t>
-  </si>
-  <si>
-    <t>ds_RNA_viral_sequence</t>
-  </si>
-  <si>
-    <t>nucleic acid</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>trif</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>TRIF</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>Gene Product</t>
-  </si>
-  <si>
-    <t>PRO:000001749</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>Trf3</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>TRAF 3</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>PRO:000002289</t>
-  </si>
-  <si>
-    <t>TANK</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>PRO:submitted</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>TBK1</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>PRO:000001779</t>
-  </si>
-  <si>
-    <t>IKKe</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>IKK-E</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>PRO:000001778</t>
-  </si>
-  <si>
-    <t>IRF3</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>IRF-3</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>PRO:000002045</t>
-  </si>
-  <si>
-    <t>2TLR3dsRNATRIFTRF3TBK1-tank-IKKe where tank is k63 ubiquitinated</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>post transcriptional modification</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">ub </t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>ubiquitin</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>gene product</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>PRO:000016963</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ISREb of IRF7pIRF7p  </t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>2TLR3dsRNATRIFTRF3</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>2TLR3dsRNATRIF+TRF3</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">2TLR3dsRNATRIFTRF3+TBK1-tank-IKKe </t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>Interferon regulatory factor-3-mediated activation of the interferon-sensitive response element by Toll-like receptor (TLR) 4 but not TLR3 requires the p65 subunit of NF-kappa.</t>
-  </si>
-  <si>
-    <t>PMID: 14557267</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IRF3pIRF3p translocate to nucleus </t>
-  </si>
-  <si>
-    <t>IRF3pIRF3p+IMPalpha4-&gt; IRF3pIRF3pIMPalpha4</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>complexes without process forming them</t>
-  </si>
-  <si>
-    <t>has_part</t>
-  </si>
-  <si>
-    <t>TBK1+tank+IKKe</t>
-  </si>
-  <si>
-    <t>pdsb</t>
-  </si>
-  <si>
-    <t>IRF3pIRF7pISREdnas</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>IRF7pIRF7p+ISREdnas</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>IRF7pIRF7pISREdnas</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>2TLR3dsRNATRIFTRF3TBK1tankk63ubIKKe-&gt;2TLR3dsRNATRIFTRF3+TBK1tankk63ubIKKe</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>IMPalpha4</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>Importina alpha 4</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>PRO:000009435</t>
-  </si>
-  <si>
-    <t>IRF3pIRF7pIMPalpha4</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>GO:0003725</t>
-  </si>
-  <si>
-    <t>double-stranded RNA binding</t>
-  </si>
-  <si>
-    <t>molecular function</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>dsRNAb</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>dsRNAb of TLR3 in 2TLR3</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>GO:0022618</t>
-  </si>
-  <si>
-    <t>RNA-protein complex assembly</t>
-  </si>
-  <si>
-    <t>process</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>2TLR3+dsRNA-&gt; 2TLR3dsRNA</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>2TLR3dsRNA+TRIF-&gt; 2TLR3dsRNATRIF</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>RNApca</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">2TLR3dsRNA </t>
-  </si>
-  <si>
-    <t>2TLR3+dsRNA</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>2TLR3dsRNATRIF</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2TLR3dsRNA+trif </t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>2TLR3dsRNATRIF+TRF3-&gt; 2TLR3dsRNATRIFTRF3</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>phet of IRF3p and phet of IRF7P</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>NLSsni</t>
-  </si>
-  <si>
-    <t>IRF7pIRF7p+IMPalpha4-&gt; IRF7pIRF7pIMPalpha4</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>nlsb of IMPalpha4</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>NLS-bearing substrate import into nucleus</t>
-  </si>
-  <si>
-    <t>GO:0006607</t>
-  </si>
-  <si>
-    <t>nlsb of IMPalpha4</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>NLSsni</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>double strand dna sequence         transcript_bound_by_protein</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>double strand dna sequence   bound by protein</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>SO:0000279</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>pDca</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>protein-DNA complex assembly</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>GO:0065004</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>super(s)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>tirdbp that has location endves</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>tirdb of trif and tirdb of TLR3 in 2TLR3dsRNA</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">ISREb of IRF3pIRF7p  </t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>tirdb</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">tir domain binding </t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>function</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>GO:0070976</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>tirdbp</t>
-  </si>
-  <si>
-    <t>tir domain complex assembly</t>
-  </si>
-  <si>
-    <t>GO:0071523</t>
-  </si>
-  <si>
-    <t>ubb</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>ubiquitin binding</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>GO:0043130</t>
-  </si>
-  <si>
-    <t>Kb</t>
-  </si>
-  <si>
-    <t>kinase binding</t>
-  </si>
-  <si>
-    <t>GO:0019900</t>
-  </si>
-  <si>
-    <t>Ka</t>
-  </si>
-  <si>
-    <t>kinase activity</t>
-  </si>
-  <si>
-    <t>GO:0016301</t>
-  </si>
-  <si>
-    <t>sf</t>
-  </si>
-  <si>
-    <t>separeted from</t>
-  </si>
-  <si>
-    <t>quality</t>
-  </si>
-  <si>
-    <t>PATO:0001505</t>
-  </si>
-  <si>
-    <t>KD</t>
-  </si>
-  <si>
-    <t>kinase domain</t>
-  </si>
-  <si>
-    <t>Ka of IKKe in TBK1tankk63ubIKKeIRF3 and Kb of IRF3 in TBK1tankk63ubIKKeIRF3</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>TBK1tankk63ubIKKeIRF3p-&gt; TBK1tankk63ubIKKe+IRF3p</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">2TLR3dsRNATRIFTRF3TBK1tankIKKe </t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>TBK1tankk63ubIKKeIRF7p-&gt; TBK1tankk63ubIKKe+IRF7p</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>PMID: 17327220   12133833</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>2TLR3dsRNATRIFTRF3TBK1tankk63ubIKKe</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>2TLR3dsRNATRIFTRF3+TBK1tankIKKe-&gt;2TLR3dsRNATRIFTRF3TBK1tankIKKe</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>2TLR3dsRNATRIFTRF3TBK1tankIKKe+ub-&gt; 2TLR3dsRNATRIFTRF3TBK1tankk63ubIKKe</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>TBK1TankIKKe</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>TBK1tankk63ubIKKeIRF3</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>TBK1tankk63ubIKKe+IRF3-&gt;TBK1tankk63ubIKKeIRF3</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>TBK1tankk63ubIKKe+IRF7-&gt;TBK1tankk63ubIKKeIRF7</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>TBK1tankk63ubIKKe+IRF3</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>TBK1tankk63ubIKKeIRF3p</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>TBK1tankk63ubIKKeIRF7</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>TBK1tankk63ubIKKeIRF7p</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>TBK1tankk63ubIKKe+IRF7</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>TBK1tankk63ubIKKeIRF7 where IRF7 is phosphorylated</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>TBK1tankk63ubIKKeIRF3 where IRF3 is phosphorylated</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>TBK1tankk63ubIKKeIRF3-&gt; TBK1tankk63ubIKKeIRF3p</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>pb</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">protein binding </t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>GO:0005515</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>pb of IRF3 and pb of TBK1 in TBK1tankk63ubIKKe</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>pca located in cyto</t>
-  </si>
-  <si>
-    <t>pca located in cyto</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>pb of IRF7 and pb of TBK1 in TBK1tankk63ubIKKe</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve"> Ka of IKKe in TBK1tankk63ubIKKeIRF7 and Kb of IRF7 in TBK1tankk63ubIKKeIRF7</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>TBK1tankk63ubIKKeIRF7-&gt; TBK1tankk63ubIKKeIRF7p</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>phom of IRF7p</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>pca located in cyto</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>pca located in cyto</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>trafdp located in eendo</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>nlsb</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>nuclear localization sequence binding</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>GO:0008139</t>
-  </si>
-  <si>
-    <t>IRF3pIRF3p+IMPalpha4</t>
-  </si>
-  <si>
-    <t>IRF7pIRF7p+IMPalpha4</t>
-  </si>
-  <si>
-    <t>IRF3pIRF7p+IMPalpha4-&gt;IRF3pIRF7pIMPalpha4</t>
-  </si>
-  <si>
-    <t>IRF3pIRF3pIMPalpha4+ISREdnas-&gt;IRF3pIRF3pISREdnas+IMPalpha4</t>
-  </si>
-  <si>
-    <t>IRF7pIRF7pIMPalpha4+ISREdnas-&gt;IRF7pIRF7pISREdnas+IMPalpha4</t>
-  </si>
-  <si>
-    <t>IRF3pIRF7pIMPalpha4+ISREdnas-&gt;IRF3pIRF7pISREdnas+IMPalpha4</t>
-  </si>
-  <si>
-    <t>IRF3pIRF7p+IMPalpha4</t>
   </si>
 </sst>
 </file>
@@ -1602,10 +1617,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
-  <dimension ref="A1:AZ101"/>
+  <dimension ref="A1:AZ102"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
+      <selection activeCell="B68" sqref="B68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -1621,29 +1636,29 @@
   <sheetData>
     <row r="1" spans="1:7" s="9" customFormat="1">
       <c r="A1" s="1" t="s">
-        <v>62</v>
+        <v>173</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>63</v>
+        <v>174</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>64</v>
+        <v>175</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>65</v>
+        <v>176</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>66</v>
+        <v>177</v>
       </c>
       <c r="F1" s="4"/>
       <c r="G1" s="4"/>
     </row>
     <row r="2" spans="1:7" ht="26">
       <c r="A2" s="5" t="s">
-        <v>11</v>
+        <v>247</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>12</v>
+        <v>248</v>
       </c>
       <c r="C2" s="7">
         <v>38707</v>
@@ -1652,14 +1667,14 @@
         <v>38383</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>138</v>
+        <v>115</v>
       </c>
       <c r="F2" s="8"/>
       <c r="G2" s="5"/>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="4" t="s">
-        <v>10</v>
+        <v>246</v>
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
@@ -1669,274 +1684,274 @@
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="1" t="s">
-        <v>67</v>
+        <v>178</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>68</v>
+        <v>179</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>69</v>
+        <v>180</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>70</v>
+        <v>181</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>71</v>
+        <v>182</v>
       </c>
       <c r="F4" s="6"/>
     </row>
     <row r="5" spans="1:7" ht="26">
       <c r="A5" s="4" t="s">
-        <v>7</v>
+        <v>243</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>140</v>
+        <v>117</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>48</v>
+        <v>284</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>139</v>
+        <v>116</v>
       </c>
       <c r="E5" s="4"/>
       <c r="F5" s="6"/>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="4" t="s">
-        <v>8</v>
+        <v>244</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>141</v>
+        <v>118</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>142</v>
+        <v>119</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>50</v>
+        <v>286</v>
       </c>
       <c r="E6" s="4"/>
       <c r="F6" s="6"/>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="4" t="s">
-        <v>9</v>
+        <v>245</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>144</v>
+        <v>121</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>145</v>
+        <v>122</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>143</v>
+        <v>120</v>
       </c>
       <c r="E7" s="4"/>
       <c r="F7" s="6"/>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="4" t="s">
-        <v>200</v>
+        <v>50</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>201</v>
+        <v>51</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>142</v>
+        <v>119</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>49</v>
+        <v>285</v>
       </c>
       <c r="E8" s="4"/>
       <c r="F8" s="6"/>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" s="4" t="s">
-        <v>202</v>
+        <v>52</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>203</v>
+        <v>53</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>142</v>
+        <v>119</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>49</v>
+        <v>285</v>
       </c>
       <c r="E9" s="4"/>
       <c r="F9" s="6"/>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="4" t="s">
-        <v>170</v>
+        <v>147</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>171</v>
+        <v>148</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>142</v>
+        <v>119</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>49</v>
+        <v>285</v>
       </c>
       <c r="E10" s="4"/>
       <c r="F10" s="6"/>
     </row>
     <row r="11" spans="1:7" ht="26">
       <c r="A11" s="4" t="s">
-        <v>247</v>
+        <v>97</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>172</v>
+        <v>149</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>142</v>
+        <v>119</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>49</v>
+        <v>285</v>
       </c>
       <c r="E11" s="4"/>
       <c r="F11" s="6"/>
     </row>
     <row r="12" spans="1:7" ht="26">
       <c r="A12" s="21" t="s">
-        <v>185</v>
+        <v>162</v>
       </c>
       <c r="B12" s="21" t="s">
-        <v>186</v>
+        <v>163</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>148</v>
+        <v>125</v>
       </c>
       <c r="D12" s="21" t="s">
-        <v>187</v>
+        <v>164</v>
       </c>
       <c r="E12" s="4"/>
       <c r="F12" s="6"/>
     </row>
     <row r="13" spans="1:7" ht="26">
       <c r="A13" s="4" t="s">
-        <v>16</v>
+        <v>252</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>13</v>
+        <v>249</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>14</v>
+        <v>250</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>15</v>
+        <v>251</v>
       </c>
       <c r="E13" s="4"/>
       <c r="F13" s="6"/>
     </row>
     <row r="14" spans="1:7" ht="26">
       <c r="A14" s="4" t="s">
-        <v>192</v>
+        <v>42</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>190</v>
+        <v>40</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>191</v>
+        <v>41</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>189</v>
+        <v>166</v>
       </c>
       <c r="E14" s="4"/>
       <c r="F14" s="6"/>
     </row>
     <row r="15" spans="1:7" ht="26">
       <c r="A15" s="4" t="s">
-        <v>265</v>
+        <v>12</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>266</v>
+        <v>13</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>134</v>
+        <v>111</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>267</v>
+        <v>14</v>
       </c>
       <c r="E15" s="4"/>
       <c r="F15" s="6"/>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" s="4" t="s">
-        <v>18</v>
+        <v>254</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>81</v>
+        <v>192</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>14</v>
+        <v>250</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>17</v>
+        <v>253</v>
       </c>
       <c r="E16" s="4"/>
       <c r="F16" s="6"/>
     </row>
     <row r="17" spans="1:10">
       <c r="A17" s="4" t="s">
-        <v>80</v>
+        <v>191</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>78</v>
+        <v>189</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>101</v>
+        <v>212</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>79</v>
+        <v>190</v>
       </c>
       <c r="E17" s="4"/>
       <c r="F17" s="6"/>
     </row>
     <row r="18" spans="1:10" ht="26">
       <c r="A18" s="4" t="s">
-        <v>104</v>
+        <v>215</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>103</v>
+        <v>214</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>101</v>
+        <v>212</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>102</v>
+        <v>213</v>
       </c>
       <c r="E18" s="4"/>
       <c r="F18" s="6"/>
     </row>
     <row r="19" spans="1:10" ht="26">
       <c r="A19" s="4" t="s">
-        <v>165</v>
+        <v>142</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>166</v>
+        <v>143</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>167</v>
+        <v>144</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>168</v>
+        <v>145</v>
       </c>
       <c r="E19" s="4"/>
       <c r="F19" s="6"/>
     </row>
     <row r="20" spans="1:10" s="9" customFormat="1" ht="13" customHeight="1">
       <c r="A20" s="4" t="s">
-        <v>146</v>
+        <v>123</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>147</v>
+        <v>124</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>148</v>
+        <v>125</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>149</v>
+        <v>126</v>
       </c>
       <c r="E20" s="15"/>
       <c r="F20" s="4"/>
@@ -1947,16 +1962,16 @@
     </row>
     <row r="21" spans="1:10" s="9" customFormat="1" ht="26">
       <c r="A21" s="11" t="s">
-        <v>150</v>
+        <v>127</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>151</v>
+        <v>128</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>148</v>
+        <v>125</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>152</v>
+        <v>129</v>
       </c>
       <c r="E21" s="4"/>
       <c r="F21" s="4"/>
@@ -1965,16 +1980,16 @@
     </row>
     <row r="22" spans="1:10" s="9" customFormat="1">
       <c r="A22" s="11" t="s">
-        <v>153</v>
+        <v>130</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>153</v>
+        <v>130</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>148</v>
+        <v>125</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>154</v>
+        <v>131</v>
       </c>
       <c r="E22" s="4"/>
       <c r="F22" s="4"/>
@@ -1983,16 +1998,16 @@
     </row>
     <row r="23" spans="1:10" s="9" customFormat="1" ht="26">
       <c r="A23" s="11" t="s">
-        <v>155</v>
+        <v>132</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>155</v>
+        <v>132</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>148</v>
+        <v>125</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>156</v>
+        <v>133</v>
       </c>
       <c r="E23" s="4"/>
       <c r="F23" s="4"/>
@@ -2001,16 +2016,16 @@
     </row>
     <row r="24" spans="1:10" s="9" customFormat="1" ht="26">
       <c r="A24" s="4" t="s">
-        <v>278</v>
+        <v>25</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>279</v>
+        <v>26</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>134</v>
+        <v>111</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>280</v>
+        <v>27</v>
       </c>
       <c r="E24" s="4"/>
       <c r="F24" s="4"/>
@@ -2019,16 +2034,16 @@
     </row>
     <row r="25" spans="1:10" s="9" customFormat="1" ht="26">
       <c r="A25" s="11" t="s">
-        <v>157</v>
+        <v>134</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>158</v>
+        <v>135</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>148</v>
+        <v>125</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>159</v>
+        <v>136</v>
       </c>
       <c r="E25" s="4"/>
       <c r="F25" s="4"/>
@@ -2037,16 +2052,16 @@
     </row>
     <row r="26" spans="1:10" s="9" customFormat="1" ht="26">
       <c r="A26" s="11" t="s">
-        <v>160</v>
+        <v>137</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>161</v>
+        <v>138</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>148</v>
+        <v>125</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>162</v>
+        <v>139</v>
       </c>
       <c r="E26" s="4"/>
       <c r="F26" s="4"/>
@@ -2055,16 +2070,16 @@
     </row>
     <row r="27" spans="1:10" s="9" customFormat="1" ht="26">
       <c r="A27" s="11" t="s">
-        <v>28</v>
+        <v>264</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>29</v>
+        <v>265</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>148</v>
+        <v>125</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>30</v>
+        <v>266</v>
       </c>
       <c r="E27" s="4"/>
       <c r="F27" s="4"/>
@@ -2073,16 +2088,16 @@
     </row>
     <row r="28" spans="1:10" s="9" customFormat="1" ht="39">
       <c r="A28" s="11" t="s">
-        <v>31</v>
+        <v>267</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>32</v>
+        <v>268</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>33</v>
+        <v>269</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>154</v>
+        <v>131</v>
       </c>
       <c r="E28" s="4"/>
       <c r="F28" s="4"/>
@@ -2091,16 +2106,16 @@
     </row>
     <row r="29" spans="1:10" s="9" customFormat="1" ht="39">
       <c r="A29" s="11" t="s">
-        <v>34</v>
+        <v>270</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>35</v>
+        <v>271</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>33</v>
+        <v>269</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>36</v>
+        <v>272</v>
       </c>
       <c r="E29" s="4"/>
       <c r="F29" s="4"/>
@@ -2109,16 +2124,16 @@
     </row>
     <row r="30" spans="1:10" s="9" customFormat="1" ht="39">
       <c r="A30" s="11" t="s">
-        <v>37</v>
+        <v>273</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>38</v>
+        <v>274</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>33</v>
+        <v>269</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>39</v>
+        <v>275</v>
       </c>
       <c r="E30" s="4"/>
       <c r="F30" s="4"/>
@@ -2127,16 +2142,16 @@
     </row>
     <row r="31" spans="1:10" s="9" customFormat="1">
       <c r="A31" s="11" t="s">
-        <v>41</v>
+        <v>277</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>42</v>
+        <v>278</v>
       </c>
       <c r="C31" s="11" t="s">
-        <v>40</v>
+        <v>276</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>154</v>
+        <v>131</v>
       </c>
       <c r="E31" s="4"/>
       <c r="F31" s="4"/>
@@ -2145,16 +2160,16 @@
     </row>
     <row r="32" spans="1:10" s="9" customFormat="1">
       <c r="A32" s="11" t="s">
-        <v>25</v>
+        <v>261</v>
       </c>
       <c r="B32" s="11" t="s">
-        <v>43</v>
+        <v>279</v>
       </c>
       <c r="C32" s="11" t="s">
-        <v>40</v>
+        <v>276</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>154</v>
+        <v>131</v>
       </c>
       <c r="E32" s="4"/>
       <c r="F32" s="4"/>
@@ -2163,16 +2178,16 @@
     </row>
     <row r="33" spans="1:8" s="9" customFormat="1">
       <c r="A33" s="11" t="s">
-        <v>44</v>
+        <v>280</v>
       </c>
       <c r="B33" s="11" t="s">
-        <v>45</v>
+        <v>281</v>
       </c>
       <c r="C33" s="11" t="s">
-        <v>40</v>
+        <v>276</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>154</v>
+        <v>131</v>
       </c>
       <c r="E33" s="4"/>
       <c r="F33" s="4"/>
@@ -2181,16 +2196,16 @@
     </row>
     <row r="34" spans="1:8" s="9" customFormat="1">
       <c r="A34" s="11" t="s">
-        <v>188</v>
+        <v>165</v>
       </c>
       <c r="B34" s="11" t="s">
-        <v>287</v>
+        <v>34</v>
       </c>
       <c r="C34" s="11" t="s">
-        <v>40</v>
+        <v>276</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>154</v>
+        <v>131</v>
       </c>
       <c r="E34" s="4"/>
       <c r="F34" s="4"/>
@@ -2199,16 +2214,16 @@
     </row>
     <row r="35" spans="1:8" s="9" customFormat="1">
       <c r="A35" s="11" t="s">
-        <v>46</v>
+        <v>282</v>
       </c>
       <c r="B35" s="11" t="s">
-        <v>281</v>
+        <v>28</v>
       </c>
       <c r="C35" s="11" t="s">
-        <v>40</v>
+        <v>276</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>154</v>
+        <v>131</v>
       </c>
       <c r="E35" s="4"/>
       <c r="F35" s="4"/>
@@ -2217,16 +2232,16 @@
     </row>
     <row r="36" spans="1:8" s="9" customFormat="1">
       <c r="A36" s="11" t="s">
-        <v>117</v>
+        <v>228</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>282</v>
+        <v>29</v>
       </c>
       <c r="C36" s="11" t="s">
-        <v>40</v>
+        <v>276</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>154</v>
+        <v>131</v>
       </c>
       <c r="E36" s="4"/>
       <c r="F36" s="4"/>
@@ -2235,16 +2250,16 @@
     </row>
     <row r="37" spans="1:8" s="9" customFormat="1">
       <c r="A37" s="11" t="s">
-        <v>181</v>
+        <v>158</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>118</v>
+        <v>229</v>
       </c>
       <c r="C37" s="11" t="s">
-        <v>40</v>
+        <v>276</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>154</v>
+        <v>131</v>
       </c>
       <c r="E37" s="4"/>
       <c r="F37" s="4"/>
@@ -2253,16 +2268,16 @@
     </row>
     <row r="38" spans="1:8" s="9" customFormat="1">
       <c r="A38" s="11" t="s">
-        <v>119</v>
+        <v>230</v>
       </c>
       <c r="B38" s="11" t="s">
-        <v>120</v>
+        <v>231</v>
       </c>
       <c r="C38" s="11" t="s">
-        <v>40</v>
+        <v>276</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>154</v>
+        <v>131</v>
       </c>
       <c r="E38" s="4"/>
       <c r="F38" s="4"/>
@@ -2271,16 +2286,16 @@
     </row>
     <row r="39" spans="1:8" s="9" customFormat="1">
       <c r="A39" s="11" t="s">
-        <v>183</v>
+        <v>160</v>
       </c>
       <c r="B39" s="11" t="s">
-        <v>182</v>
+        <v>159</v>
       </c>
       <c r="C39" s="11" t="s">
-        <v>40</v>
+        <v>276</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>154</v>
+        <v>131</v>
       </c>
       <c r="E39" s="4"/>
       <c r="F39" s="4"/>
@@ -2289,16 +2304,16 @@
     </row>
     <row r="40" spans="1:8" s="9" customFormat="1">
       <c r="A40" s="11" t="s">
-        <v>121</v>
+        <v>232</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>122</v>
+        <v>233</v>
       </c>
       <c r="C40" s="11" t="s">
-        <v>40</v>
+        <v>276</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>154</v>
+        <v>131</v>
       </c>
       <c r="E40" s="4"/>
       <c r="F40" s="4"/>
@@ -2307,16 +2322,16 @@
     </row>
     <row r="41" spans="1:8" s="9" customFormat="1" ht="39">
       <c r="A41" s="11" t="s">
-        <v>250</v>
+        <v>100</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>163</v>
+        <v>140</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>164</v>
+        <v>141</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>154</v>
+        <v>131</v>
       </c>
       <c r="E41" s="4"/>
       <c r="F41" s="4"/>
@@ -2325,16 +2340,16 @@
     </row>
     <row r="42" spans="1:8" s="9" customFormat="1">
       <c r="A42" s="4" t="s">
-        <v>124</v>
+        <v>235</v>
       </c>
       <c r="B42" s="11" t="s">
-        <v>125</v>
+        <v>102</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>40</v>
+        <v>276</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>154</v>
+        <v>131</v>
       </c>
       <c r="E42" s="4"/>
       <c r="F42" s="4"/>
@@ -2343,16 +2358,16 @@
     </row>
     <row r="43" spans="1:8" s="9" customFormat="1" ht="39">
       <c r="A43" s="4" t="s">
-        <v>126</v>
+        <v>103</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>127</v>
+        <v>104</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>123</v>
+        <v>234</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>154</v>
+        <v>131</v>
       </c>
       <c r="E43" s="4"/>
       <c r="F43" s="4"/>
@@ -2361,16 +2376,16 @@
     </row>
     <row r="44" spans="1:8" s="9" customFormat="1">
       <c r="A44" s="4" t="s">
-        <v>254</v>
+        <v>1</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>257</v>
+        <v>4</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>40</v>
+        <v>276</v>
       </c>
       <c r="D44" s="4" t="s">
-        <v>154</v>
+        <v>131</v>
       </c>
       <c r="E44" s="4"/>
       <c r="F44" s="4"/>
@@ -2379,16 +2394,16 @@
     </row>
     <row r="45" spans="1:8" s="9" customFormat="1" ht="39">
       <c r="A45" s="4" t="s">
-        <v>258</v>
+        <v>5</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>263</v>
+        <v>10</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>123</v>
+        <v>234</v>
       </c>
       <c r="D45" s="4" t="s">
-        <v>154</v>
+        <v>131</v>
       </c>
       <c r="E45" s="4"/>
       <c r="F45" s="4"/>
@@ -2397,16 +2412,16 @@
     </row>
     <row r="46" spans="1:8" s="9" customFormat="1">
       <c r="A46" s="4" t="s">
-        <v>259</v>
+        <v>6</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>261</v>
+        <v>8</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>40</v>
+        <v>276</v>
       </c>
       <c r="D46" s="4" t="s">
-        <v>154</v>
+        <v>131</v>
       </c>
       <c r="E46" s="4"/>
       <c r="F46" s="4"/>
@@ -2415,16 +2430,16 @@
     </row>
     <row r="47" spans="1:8" s="9" customFormat="1" ht="39">
       <c r="A47" s="4" t="s">
-        <v>260</v>
+        <v>7</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>262</v>
+        <v>9</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>123</v>
+        <v>234</v>
       </c>
       <c r="D47" s="4" t="s">
-        <v>154</v>
+        <v>131</v>
       </c>
       <c r="E47" s="4"/>
       <c r="F47" s="4"/>
@@ -2433,16 +2448,16 @@
     </row>
     <row r="48" spans="1:8" s="9" customFormat="1" ht="26">
       <c r="A48" s="4" t="s">
-        <v>128</v>
+        <v>105</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>129</v>
+        <v>106</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>130</v>
+        <v>107</v>
       </c>
       <c r="D48" s="4" t="s">
-        <v>131</v>
+        <v>108</v>
       </c>
       <c r="E48" s="4"/>
       <c r="F48" s="4"/>
@@ -2451,16 +2466,16 @@
     </row>
     <row r="49" spans="1:52" s="9" customFormat="1" ht="26">
       <c r="A49" s="11" t="s">
-        <v>132</v>
+        <v>109</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>133</v>
+        <v>110</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>134</v>
+        <v>111</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>135</v>
+        <v>112</v>
       </c>
       <c r="E49" s="4"/>
       <c r="F49" s="4"/>
@@ -2469,16 +2484,16 @@
     </row>
     <row r="50" spans="1:52" s="9" customFormat="1" ht="26">
       <c r="A50" s="11" t="s">
-        <v>86</v>
+        <v>197</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>87</v>
+        <v>198</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>88</v>
+        <v>199</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>136</v>
+        <v>113</v>
       </c>
       <c r="E50" s="4"/>
       <c r="F50" s="4"/>
@@ -2487,16 +2502,16 @@
     </row>
     <row r="51" spans="1:52" s="9" customFormat="1" ht="26">
       <c r="A51" s="11" t="s">
-        <v>89</v>
+        <v>200</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>90</v>
+        <v>201</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>88</v>
+        <v>199</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>91</v>
+        <v>202</v>
       </c>
       <c r="E51" s="4"/>
       <c r="F51" s="4"/>
@@ -2505,16 +2520,16 @@
     </row>
     <row r="52" spans="1:52" s="9" customFormat="1">
       <c r="A52" s="11" t="s">
-        <v>92</v>
+        <v>203</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>93</v>
+        <v>204</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>94</v>
+        <v>205</v>
       </c>
       <c r="D52" s="4" t="s">
-        <v>95</v>
+        <v>206</v>
       </c>
       <c r="E52" s="4"/>
       <c r="F52" s="4"/>
@@ -2523,16 +2538,16 @@
     </row>
     <row r="53" spans="1:52" s="9" customFormat="1" ht="27" customHeight="1">
       <c r="A53" s="9" t="s">
-        <v>96</v>
+        <v>207</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>84</v>
+        <v>195</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>94</v>
+        <v>205</v>
       </c>
       <c r="D53" s="4" t="s">
-        <v>97</v>
+        <v>208</v>
       </c>
       <c r="E53" s="4"/>
       <c r="F53" s="4"/>
@@ -2541,16 +2556,16 @@
     </row>
     <row r="54" spans="1:52" s="9" customFormat="1" ht="26">
       <c r="A54" s="11" t="s">
-        <v>98</v>
+        <v>209</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>99</v>
+        <v>210</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>100</v>
+        <v>211</v>
       </c>
       <c r="D54" s="4" t="s">
-        <v>112</v>
+        <v>223</v>
       </c>
       <c r="E54" s="4"/>
       <c r="F54" s="4"/>
@@ -2559,16 +2574,16 @@
     </row>
     <row r="55" spans="1:52" s="9" customFormat="1" ht="26">
       <c r="A55" s="4" t="s">
-        <v>206</v>
+        <v>56</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>209</v>
+        <v>59</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>85</v>
+        <v>196</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>210</v>
+        <v>60</v>
       </c>
       <c r="E55" s="17"/>
       <c r="F55" s="17"/>
@@ -2621,16 +2636,16 @@
     </row>
     <row r="56" spans="1:52" s="9" customFormat="1" ht="26">
       <c r="A56" s="11" t="s">
-        <v>113</v>
+        <v>224</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>114</v>
+        <v>225</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>100</v>
+        <v>211</v>
       </c>
       <c r="D56" s="4" t="s">
-        <v>115</v>
+        <v>226</v>
       </c>
       <c r="E56" s="4"/>
       <c r="F56" s="4"/>
@@ -2639,16 +2654,16 @@
     </row>
     <row r="57" spans="1:52" s="9" customFormat="1" ht="26">
       <c r="A57" s="11" t="s">
-        <v>199</v>
+        <v>49</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>195</v>
+        <v>45</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>196</v>
+        <v>46</v>
       </c>
       <c r="D57" s="4" t="s">
-        <v>194</v>
+        <v>44</v>
       </c>
       <c r="E57" s="4"/>
       <c r="F57" s="4"/>
@@ -2657,16 +2672,16 @@
     </row>
     <row r="58" spans="1:52" s="9" customFormat="1" ht="52">
       <c r="A58" s="4" t="s">
-        <v>116</v>
+        <v>227</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>213</v>
+        <v>63</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>214</v>
+        <v>64</v>
       </c>
       <c r="D58" s="4" t="s">
-        <v>215</v>
+        <v>65</v>
       </c>
       <c r="E58" s="4"/>
       <c r="F58" s="4"/>
@@ -2675,16 +2690,16 @@
     </row>
     <row r="59" spans="1:52" s="9" customFormat="1" ht="26">
       <c r="A59" s="5" t="s">
-        <v>216</v>
+        <v>66</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>217</v>
+        <v>67</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>100</v>
+        <v>211</v>
       </c>
       <c r="D59" s="4" t="s">
-        <v>218</v>
+        <v>68</v>
       </c>
       <c r="E59" s="4"/>
       <c r="F59" s="4"/>
@@ -2693,16 +2708,16 @@
     </row>
     <row r="60" spans="1:52" s="9" customFormat="1">
       <c r="A60" s="4" t="s">
-        <v>243</v>
+        <v>93</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>244</v>
+        <v>94</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>110</v>
+        <v>221</v>
       </c>
       <c r="D60" s="4" t="s">
-        <v>111</v>
+        <v>222</v>
       </c>
       <c r="E60" s="4"/>
       <c r="F60" s="4"/>
@@ -2755,16 +2770,16 @@
     </row>
     <row r="61" spans="1:52" s="9" customFormat="1" ht="12" customHeight="1">
       <c r="A61" s="4" t="s">
-        <v>233</v>
+        <v>83</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>234</v>
+        <v>84</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>130</v>
+        <v>107</v>
       </c>
       <c r="D61" s="4" t="s">
-        <v>235</v>
+        <v>85</v>
       </c>
       <c r="E61" s="17"/>
       <c r="F61" s="17"/>
@@ -2817,16 +2832,16 @@
     </row>
     <row r="62" spans="1:52" s="9" customFormat="1" ht="26">
       <c r="A62" s="4" t="s">
-        <v>236</v>
+        <v>86</v>
       </c>
       <c r="B62" s="4" t="s">
-        <v>237</v>
+        <v>87</v>
       </c>
       <c r="C62" s="4" t="s">
-        <v>130</v>
+        <v>107</v>
       </c>
       <c r="D62" s="4" t="s">
-        <v>238</v>
+        <v>88</v>
       </c>
       <c r="E62" s="17"/>
       <c r="F62" s="17"/>
@@ -2879,16 +2894,16 @@
     </row>
     <row r="63" spans="1:52" s="9" customFormat="1">
       <c r="A63" s="4" t="s">
-        <v>239</v>
+        <v>89</v>
       </c>
       <c r="B63" s="4" t="s">
-        <v>240</v>
+        <v>90</v>
       </c>
       <c r="C63" s="4" t="s">
-        <v>241</v>
+        <v>91</v>
       </c>
       <c r="D63" s="4" t="s">
-        <v>242</v>
+        <v>92</v>
       </c>
       <c r="E63" s="17"/>
       <c r="F63" s="17"/>
@@ -2941,16 +2956,16 @@
     </row>
     <row r="64" spans="1:52" s="19" customFormat="1">
       <c r="A64" s="4" t="s">
-        <v>223</v>
+        <v>73</v>
       </c>
       <c r="B64" s="4" t="s">
-        <v>224</v>
+        <v>74</v>
       </c>
       <c r="C64" s="4" t="s">
-        <v>225</v>
+        <v>75</v>
       </c>
       <c r="D64" s="4" t="s">
-        <v>226</v>
+        <v>76</v>
       </c>
       <c r="E64" s="4"/>
       <c r="F64" s="6"/>
@@ -2959,16 +2974,16 @@
     </row>
     <row r="65" spans="1:8" s="19" customFormat="1" ht="26">
       <c r="A65" s="4" t="s">
-        <v>230</v>
+        <v>80</v>
       </c>
       <c r="B65" s="4" t="s">
-        <v>231</v>
+        <v>81</v>
       </c>
       <c r="C65" s="4" t="s">
-        <v>134</v>
+        <v>111</v>
       </c>
       <c r="D65" s="4" t="s">
-        <v>232</v>
+        <v>82</v>
       </c>
       <c r="E65" s="4"/>
       <c r="F65" s="6"/>
@@ -2977,133 +2992,139 @@
     </row>
     <row r="66" spans="1:8" s="19" customFormat="1" ht="26">
       <c r="A66" s="9" t="s">
-        <v>227</v>
+        <v>77</v>
       </c>
       <c r="B66" s="4" t="s">
-        <v>228</v>
+        <v>78</v>
       </c>
       <c r="C66" s="9" t="s">
-        <v>85</v>
+        <v>196</v>
       </c>
       <c r="D66" s="9" t="s">
-        <v>229</v>
+        <v>79</v>
       </c>
       <c r="E66" s="4"/>
       <c r="F66" s="6"/>
       <c r="G66" s="4"/>
       <c r="H66" s="18"/>
     </row>
-    <row r="67" spans="1:8" ht="26">
-      <c r="A67" s="4"/>
-      <c r="B67" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C67" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="D67" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="E67" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="F67" s="20" t="s">
-        <v>219</v>
-      </c>
-      <c r="G67" s="1" t="s">
-        <v>74</v>
-      </c>
+    <row r="67" spans="1:8" s="19" customFormat="1">
+      <c r="A67" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B67" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C67" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D67" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="E67" s="4"/>
+      <c r="F67" s="6"/>
+      <c r="G67" s="4"/>
+      <c r="H67" s="18"/>
     </row>
     <row r="68" spans="1:8" ht="26">
       <c r="A68" s="4"/>
-      <c r="B68" s="4" t="s">
-        <v>197</v>
-      </c>
-      <c r="C68" s="4" t="s">
-        <v>193</v>
-      </c>
-      <c r="D68" s="11" t="s">
-        <v>199</v>
-      </c>
-      <c r="E68" s="4"/>
-      <c r="F68" s="6"/>
-      <c r="G68" s="4" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="69" spans="1:8" ht="39">
+      <c r="B68" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="D68" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="E68" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="F68" s="20" t="s">
+        <v>69</v>
+      </c>
+      <c r="G68" s="1" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" ht="26">
       <c r="A69" s="4"/>
       <c r="B69" s="4" t="s">
-        <v>198</v>
-      </c>
-      <c r="C69" s="21" t="s">
-        <v>221</v>
-      </c>
-      <c r="D69" s="4" t="s">
-        <v>220</v>
+        <v>47</v>
+      </c>
+      <c r="C69" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D69" s="11" t="s">
+        <v>49</v>
       </c>
       <c r="E69" s="4"/>
       <c r="F69" s="6"/>
       <c r="G69" s="4" t="s">
-        <v>76</v>
+        <v>186</v>
       </c>
     </row>
     <row r="70" spans="1:8" ht="39">
       <c r="A70" s="4"/>
       <c r="B70" s="4" t="s">
-        <v>204</v>
-      </c>
-      <c r="C70" s="4" t="s">
-        <v>82</v>
+        <v>48</v>
+      </c>
+      <c r="C70" s="21" t="s">
+        <v>71</v>
       </c>
       <c r="D70" s="4" t="s">
-        <v>19</v>
+        <v>70</v>
       </c>
       <c r="E70" s="4"/>
-      <c r="F70" s="10"/>
+      <c r="F70" s="6"/>
       <c r="G70" s="4" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="71" spans="1:8" ht="52">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" ht="39">
       <c r="A71" s="4"/>
       <c r="B71" s="4" t="s">
-        <v>251</v>
+        <v>54</v>
       </c>
       <c r="C71" s="4" t="s">
-        <v>20</v>
+        <v>193</v>
       </c>
       <c r="D71" s="4" t="s">
-        <v>277</v>
+        <v>255</v>
       </c>
       <c r="E71" s="4"/>
-      <c r="F71" s="6"/>
+      <c r="F71" s="10"/>
       <c r="G71" s="4" t="s">
-        <v>77</v>
+        <v>188</v>
       </c>
     </row>
     <row r="72" spans="1:8" ht="52">
       <c r="A72" s="4"/>
       <c r="B72" s="4" t="s">
-        <v>252</v>
-      </c>
-      <c r="C72" s="11" t="s">
-        <v>27</v>
+        <v>101</v>
+      </c>
+      <c r="C72" s="4" t="s">
+        <v>256</v>
       </c>
       <c r="D72" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E72" s="4"/>
       <c r="F72" s="6"/>
+      <c r="G72" s="4" t="s">
+        <v>188</v>
+      </c>
     </row>
     <row r="73" spans="1:8" ht="52">
       <c r="A73" s="4"/>
       <c r="B73" s="4" t="s">
-        <v>184</v>
-      </c>
-      <c r="C73" s="11"/>
+        <v>0</v>
+      </c>
+      <c r="C73" s="11" t="s">
+        <v>263</v>
+      </c>
       <c r="D73" s="4" t="s">
-        <v>83</v>
+        <v>262</v>
       </c>
       <c r="E73" s="4"/>
       <c r="F73" s="6"/>
@@ -3111,91 +3132,89 @@
     <row r="74" spans="1:8" ht="52">
       <c r="A74" s="4"/>
       <c r="B74" s="4" t="s">
-        <v>255</v>
-      </c>
-      <c r="C74" s="11" t="s">
-        <v>268</v>
-      </c>
+        <v>161</v>
+      </c>
+      <c r="C74" s="11"/>
       <c r="D74" s="4" t="s">
-        <v>270</v>
+        <v>194</v>
       </c>
       <c r="E74" s="4"/>
       <c r="F74" s="6"/>
     </row>
-    <row r="75" spans="1:8" ht="78">
+    <row r="75" spans="1:8" ht="52">
       <c r="A75" s="4"/>
       <c r="B75" s="4" t="s">
-        <v>264</v>
-      </c>
-      <c r="C75" s="4" t="s">
-        <v>245</v>
+        <v>2</v>
+      </c>
+      <c r="C75" s="11" t="s">
+        <v>15</v>
       </c>
       <c r="D75" s="4" t="s">
-        <v>47</v>
+        <v>17</v>
       </c>
       <c r="E75" s="4"/>
       <c r="F75" s="6"/>
     </row>
-    <row r="76" spans="1:8" ht="26">
+    <row r="76" spans="1:8" ht="78">
       <c r="A76" s="4"/>
-      <c r="B76" s="2" t="s">
-        <v>246</v>
+      <c r="B76" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C76" s="4" t="s">
+        <v>95</v>
       </c>
       <c r="D76" s="4" t="s">
-        <v>83</v>
+        <v>283</v>
       </c>
       <c r="E76" s="4"/>
       <c r="F76" s="6"/>
     </row>
-    <row r="77" spans="1:8" ht="55" customHeight="1">
+    <row r="77" spans="1:8" ht="26">
       <c r="A77" s="4"/>
-      <c r="B77" s="4" t="s">
-        <v>256</v>
-      </c>
-      <c r="C77" s="4" t="s">
-        <v>271</v>
+      <c r="B77" s="2" t="s">
+        <v>96</v>
       </c>
       <c r="D77" s="4" t="s">
-        <v>269</v>
+        <v>194</v>
       </c>
       <c r="E77" s="4"/>
       <c r="F77" s="6"/>
     </row>
-    <row r="78" spans="1:8" ht="78">
+    <row r="78" spans="1:8" ht="55" customHeight="1">
       <c r="A78" s="4"/>
       <c r="B78" s="4" t="s">
-        <v>273</v>
+        <v>3</v>
       </c>
       <c r="C78" s="4" t="s">
-        <v>272</v>
+        <v>18</v>
       </c>
       <c r="D78" s="4" t="s">
-        <v>47</v>
+        <v>16</v>
       </c>
       <c r="E78" s="4"/>
       <c r="F78" s="6"/>
     </row>
-    <row r="79" spans="1:8" ht="26">
+    <row r="79" spans="1:8" ht="78">
       <c r="A79" s="4"/>
-      <c r="B79" s="2" t="s">
-        <v>248</v>
+      <c r="B79" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C79" s="4" t="s">
+        <v>19</v>
       </c>
       <c r="D79" s="4" t="s">
-        <v>83</v>
+        <v>283</v>
       </c>
       <c r="E79" s="4"/>
       <c r="F79" s="6"/>
     </row>
     <row r="80" spans="1:8" ht="26">
       <c r="A80" s="4"/>
-      <c r="B80" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="C80" s="4" t="s">
-        <v>274</v>
+      <c r="B80" s="2" t="s">
+        <v>98</v>
       </c>
       <c r="D80" s="4" t="s">
-        <v>276</v>
+        <v>194</v>
       </c>
       <c r="E80" s="4"/>
       <c r="F80" s="6"/>
@@ -3203,83 +3222,83 @@
     <row r="81" spans="1:6" ht="26">
       <c r="A81" s="4"/>
       <c r="B81" s="4" t="s">
-        <v>61</v>
+        <v>170</v>
       </c>
       <c r="C81" s="4" t="s">
         <v>21</v>
       </c>
       <c r="D81" s="4" t="s">
-        <v>60</v>
+        <v>23</v>
       </c>
       <c r="E81" s="4"/>
       <c r="F81" s="6"/>
     </row>
-    <row r="82" spans="1:6" ht="39">
+    <row r="82" spans="1:6" ht="26">
       <c r="A82" s="4"/>
       <c r="B82" s="4" t="s">
-        <v>22</v>
+        <v>172</v>
       </c>
       <c r="C82" s="4" t="s">
-        <v>205</v>
+        <v>257</v>
       </c>
       <c r="D82" s="4" t="s">
-        <v>275</v>
+        <v>171</v>
       </c>
       <c r="E82" s="4"/>
       <c r="F82" s="6"/>
     </row>
-    <row r="83" spans="1:6" ht="26">
+    <row r="83" spans="1:6" ht="39">
       <c r="A83" s="4"/>
       <c r="B83" s="4" t="s">
-        <v>176</v>
+        <v>258</v>
       </c>
       <c r="C83" s="4" t="s">
-        <v>211</v>
+        <v>55</v>
       </c>
       <c r="D83" s="4" t="s">
-        <v>212</v>
+        <v>22</v>
       </c>
       <c r="E83" s="4"/>
       <c r="F83" s="6"/>
     </row>
     <row r="84" spans="1:6" ht="26">
       <c r="A84" s="4"/>
-      <c r="B84" s="5" t="s">
-        <v>207</v>
+      <c r="B84" s="4" t="s">
+        <v>153</v>
       </c>
       <c r="C84" s="4" t="s">
-        <v>208</v>
+        <v>61</v>
       </c>
       <c r="D84" s="4" t="s">
-        <v>206</v>
+        <v>62</v>
       </c>
       <c r="E84" s="4"/>
       <c r="F84" s="6"/>
     </row>
     <row r="85" spans="1:6" ht="26">
       <c r="A85" s="4"/>
-      <c r="B85" s="4" t="s">
-        <v>283</v>
+      <c r="B85" s="5" t="s">
+        <v>57</v>
       </c>
       <c r="C85" s="4" t="s">
-        <v>211</v>
+        <v>58</v>
       </c>
       <c r="D85" s="4" t="s">
-        <v>206</v>
+        <v>56</v>
       </c>
       <c r="E85" s="4"/>
       <c r="F85" s="6"/>
     </row>
-    <row r="86" spans="1:6" ht="52">
+    <row r="86" spans="1:6" ht="26">
       <c r="A86" s="4"/>
       <c r="B86" s="4" t="s">
-        <v>284</v>
+        <v>30</v>
       </c>
       <c r="C86" s="4" t="s">
-        <v>23</v>
+        <v>61</v>
       </c>
       <c r="D86" s="4" t="s">
-        <v>24</v>
+        <v>56</v>
       </c>
       <c r="E86" s="4"/>
       <c r="F86" s="6"/>
@@ -3287,13 +3306,13 @@
     <row r="87" spans="1:6" ht="52">
       <c r="A87" s="4"/>
       <c r="B87" s="4" t="s">
-        <v>285</v>
+        <v>31</v>
       </c>
       <c r="C87" s="4" t="s">
-        <v>169</v>
+        <v>259</v>
       </c>
       <c r="D87" s="4" t="s">
-        <v>24</v>
+        <v>260</v>
       </c>
       <c r="E87" s="4"/>
       <c r="F87" s="6"/>
@@ -3301,163 +3320,177 @@
     <row r="88" spans="1:6" ht="52">
       <c r="A88" s="4"/>
       <c r="B88" s="4" t="s">
-        <v>286</v>
+        <v>32</v>
       </c>
       <c r="C88" s="4" t="s">
-        <v>222</v>
+        <v>146</v>
       </c>
       <c r="D88" s="4" t="s">
-        <v>24</v>
+        <v>260</v>
       </c>
       <c r="E88" s="4"/>
       <c r="F88" s="6"/>
     </row>
-    <row r="89" spans="1:6" ht="34" customHeight="1">
+    <row r="89" spans="1:6" ht="52">
       <c r="A89" s="4"/>
-      <c r="B89" s="22" t="s">
-        <v>177</v>
-      </c>
-      <c r="C89" s="22" t="s">
-        <v>178</v>
-      </c>
-      <c r="D89" s="5"/>
+      <c r="B89" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C89" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="D89" s="4" t="s">
+        <v>260</v>
+      </c>
       <c r="E89" s="4"/>
       <c r="F89" s="6"/>
     </row>
-    <row r="90" spans="1:6" ht="26">
+    <row r="90" spans="1:6" ht="34" customHeight="1">
       <c r="A90" s="4"/>
-      <c r="B90" s="2" t="s">
-        <v>253</v>
-      </c>
-      <c r="C90" s="2" t="s">
-        <v>179</v>
-      </c>
-      <c r="D90" s="4" t="s">
-        <v>180</v>
-      </c>
+      <c r="B90" s="22" t="s">
+        <v>154</v>
+      </c>
+      <c r="C90" s="22" t="s">
+        <v>155</v>
+      </c>
+      <c r="D90" s="5"/>
       <c r="E90" s="4"/>
       <c r="F90" s="6"/>
     </row>
-    <row r="91" spans="1:6">
-      <c r="A91" s="12" t="s">
-        <v>105</v>
-      </c>
-      <c r="B91" s="12" t="s">
-        <v>106</v>
-      </c>
-      <c r="C91" s="12" t="s">
-        <v>107</v>
-      </c>
-      <c r="D91" s="12" t="s">
-        <v>108</v>
-      </c>
-      <c r="E91" s="3" t="s">
-        <v>109</v>
-      </c>
+    <row r="91" spans="1:6" ht="26">
+      <c r="A91" s="4"/>
+      <c r="B91" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C91" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="D91" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="E91" s="4"/>
       <c r="F91" s="6"/>
     </row>
-    <row r="92" spans="1:6" ht="26">
-      <c r="A92" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="B92" s="13"/>
-      <c r="C92" s="13"/>
-      <c r="D92" s="13"/>
-      <c r="E92" s="14"/>
+    <row r="92" spans="1:6">
+      <c r="A92" s="12" t="s">
+        <v>216</v>
+      </c>
+      <c r="B92" s="12" t="s">
+        <v>217</v>
+      </c>
+      <c r="C92" s="12" t="s">
+        <v>218</v>
+      </c>
+      <c r="D92" s="12" t="s">
+        <v>219</v>
+      </c>
+      <c r="E92" s="3" t="s">
+        <v>220</v>
+      </c>
       <c r="F92" s="6"/>
     </row>
-    <row r="93" spans="1:6" ht="52">
+    <row r="93" spans="1:6" ht="26">
       <c r="A93" s="4" t="s">
-        <v>56</v>
+        <v>291</v>
       </c>
       <c r="B93" s="13"/>
       <c r="C93" s="13"/>
-      <c r="D93" s="13" t="s">
-        <v>249</v>
-      </c>
+      <c r="D93" s="13"/>
       <c r="E93" s="14"/>
-    </row>
-    <row r="94" spans="1:6" ht="117">
+      <c r="F93" s="6"/>
+    </row>
+    <row r="94" spans="1:6" ht="52">
       <c r="A94" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="B94" s="13" t="s">
-        <v>0</v>
-      </c>
+        <v>167</v>
+      </c>
+      <c r="B94" s="13"/>
       <c r="C94" s="13"/>
       <c r="D94" s="13" t="s">
-        <v>1</v>
+        <v>99</v>
       </c>
       <c r="E94" s="14"/>
     </row>
-    <row r="95" spans="1:6" ht="52">
+    <row r="95" spans="1:6" ht="117">
       <c r="A95" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="B95" s="13"/>
-      <c r="C95" s="4"/>
-      <c r="D95" s="13"/>
+        <v>168</v>
+      </c>
+      <c r="B95" s="13" t="s">
+        <v>236</v>
+      </c>
+      <c r="C95" s="13"/>
+      <c r="D95" s="13" t="s">
+        <v>237</v>
+      </c>
       <c r="E95" s="14"/>
     </row>
-    <row r="96" spans="1:6" ht="65">
+    <row r="96" spans="1:6" ht="52">
       <c r="A96" s="4" t="s">
-        <v>137</v>
-      </c>
-      <c r="B96" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D96" s="2" t="s">
-        <v>3</v>
-      </c>
+        <v>169</v>
+      </c>
+      <c r="B96" s="13"/>
+      <c r="C96" s="4"/>
+      <c r="D96" s="13"/>
+      <c r="E96" s="14"/>
     </row>
     <row r="97" spans="1:4" ht="65">
       <c r="A97" s="4" t="s">
-        <v>4</v>
+        <v>114</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>2</v>
+        <v>238</v>
       </c>
       <c r="D97" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="98" spans="1:4" ht="91">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" ht="65">
       <c r="A98" s="4" t="s">
-        <v>5</v>
+        <v>240</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>173</v>
+        <v>238</v>
       </c>
       <c r="D98" s="2" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="99" spans="1:4" ht="104">
-      <c r="A99" s="5" t="s">
-        <v>175</v>
+        <v>239</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" ht="91">
+      <c r="A99" s="4" t="s">
+        <v>241</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>51</v>
+        <v>150</v>
       </c>
       <c r="D99" s="2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="100" spans="1:4">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" ht="104">
       <c r="A100" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="C100" s="4"/>
+        <v>152</v>
+      </c>
+      <c r="B100" s="2" t="s">
+        <v>287</v>
+      </c>
+      <c r="D100" s="2" t="s">
+        <v>288</v>
+      </c>
     </row>
     <row r="101" spans="1:4">
       <c r="A101" s="5" t="s">
-        <v>54</v>
+        <v>289</v>
+      </c>
+      <c r="C101" s="4"/>
+    </row>
+    <row r="102" spans="1:4">
+      <c r="A102" s="5" t="s">
+        <v>290</v>
       </c>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>